<commit_message>
improve plot colors and dashboard
</commit_message>
<xml_diff>
--- a/test_env/dashboard_creation/Databank.xlsx
+++ b/test_env/dashboard_creation/Databank.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AB72"/>
+  <dimension ref="A1:Z73"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -546,32 +546,22 @@
       </c>
       <c r="W1" s="1" t="inlineStr">
         <is>
-          <t>EU_estimate</t>
+          <t>Pax</t>
         </is>
       </c>
       <c r="X1" s="1" t="inlineStr">
         <is>
-          <t>Pax</t>
+          <t>Height,float,metre</t>
         </is>
       </c>
       <c r="Y1" s="1" t="inlineStr">
         <is>
-          <t>Height,float,metre</t>
+          <t>B/P Ratio</t>
         </is>
       </c>
       <c r="Z1" s="1" t="inlineStr">
         <is>
-          <t>B/P Ratio</t>
-        </is>
-      </c>
-      <c r="AA1" s="1" t="inlineStr">
-        <is>
           <t>Overcome Thrust</t>
-        </is>
-      </c>
-      <c r="AB1" s="1" t="inlineStr">
-        <is>
-          <t>EU_estimate_Limit</t>
         </is>
       </c>
     </row>
@@ -639,15 +629,13 @@
         <v>0.01585118999772539</v>
       </c>
       <c r="W2" t="inlineStr"/>
-      <c r="X2" t="inlineStr"/>
+      <c r="X2" t="n">
+        <v>17.11</v>
+      </c>
       <c r="Y2" t="n">
-        <v>17.11</v>
-      </c>
-      <c r="Z2" t="n">
         <v>7.5</v>
       </c>
-      <c r="AA2" t="inlineStr"/>
-      <c r="AB2" t="inlineStr"/>
+      <c r="Z2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -719,15 +707,13 @@
         <v>0.01295514424609528</v>
       </c>
       <c r="W3" t="inlineStr"/>
-      <c r="X3" t="inlineStr"/>
+      <c r="X3" t="n">
+        <v>24.09</v>
+      </c>
       <c r="Y3" t="n">
-        <v>24.09</v>
-      </c>
-      <c r="Z3" t="n">
         <v>8.348000000000001</v>
       </c>
-      <c r="AA3" t="inlineStr"/>
-      <c r="AB3" t="inlineStr"/>
+      <c r="Z3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -803,22 +789,16 @@
         <v>0.02695082003825436</v>
       </c>
       <c r="W4" t="n">
-        <v>1.14307207999559</v>
+        <v>156</v>
       </c>
       <c r="X4" t="n">
-        <v>156</v>
+        <v>11.76</v>
       </c>
       <c r="Y4" t="n">
-        <v>11.76</v>
+        <v>5.694166666666667</v>
       </c>
       <c r="Z4" t="n">
-        <v>5.694166666666667</v>
-      </c>
-      <c r="AA4" t="n">
         <v>58401.1920317827</v>
-      </c>
-      <c r="AB4" t="n">
-        <v>0.914457663996472</v>
       </c>
     </row>
     <row r="5">
@@ -884,20 +864,18 @@
       <c r="T5" t="inlineStr"/>
       <c r="U5" t="inlineStr"/>
       <c r="V5" t="inlineStr"/>
-      <c r="W5" t="inlineStr"/>
+      <c r="W5" t="n">
+        <v>118</v>
+      </c>
       <c r="X5" t="n">
-        <v>118</v>
+        <v>12.79</v>
       </c>
       <c r="Y5" t="n">
-        <v>12.79</v>
+        <v>5.566666666666666</v>
       </c>
       <c r="Z5" t="n">
-        <v>5.566666666666666</v>
-      </c>
-      <c r="AA5" t="n">
         <v>53222.18275336444</v>
       </c>
-      <c r="AB5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -973,22 +951,16 @@
         <v>0.02921086162158479</v>
       </c>
       <c r="W6" t="n">
-        <v>1.531120491263444</v>
+        <v>261</v>
       </c>
       <c r="X6" t="n">
-        <v>261</v>
+        <v>16.66</v>
       </c>
       <c r="Y6" t="n">
-        <v>16.66</v>
+        <v>4.938461538461539</v>
       </c>
       <c r="Z6" t="n">
-        <v>4.938461538461539</v>
-      </c>
-      <c r="AA6" t="n">
         <v>122660.0008671653</v>
-      </c>
-      <c r="AB6" t="n">
-        <v>1.158325936868866</v>
       </c>
     </row>
     <row r="7">
@@ -1050,20 +1022,18 @@
       <c r="T7" t="inlineStr"/>
       <c r="U7" t="inlineStr"/>
       <c r="V7" t="inlineStr"/>
-      <c r="W7" t="inlineStr"/>
+      <c r="W7" t="n">
+        <v>255</v>
+      </c>
       <c r="X7" t="n">
-        <v>255</v>
+        <v>16.72</v>
       </c>
       <c r="Y7" t="n">
-        <v>16.72</v>
+        <v>4.366666666666666</v>
       </c>
       <c r="Z7" t="n">
-        <v>4.366666666666666</v>
-      </c>
-      <c r="AA7" t="n">
         <v>163347.4258846782</v>
       </c>
-      <c r="AB7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1124,18 +1094,16 @@
       <c r="T8" t="inlineStr"/>
       <c r="U8" t="inlineStr"/>
       <c r="V8" t="inlineStr"/>
-      <c r="W8" t="inlineStr"/>
+      <c r="W8" t="n">
+        <v>179</v>
+      </c>
       <c r="X8" t="n">
-        <v>179</v>
+        <v>15.95</v>
       </c>
       <c r="Y8" t="n">
-        <v>15.95</v>
-      </c>
-      <c r="Z8" t="n">
         <v>5.033333333333333</v>
       </c>
-      <c r="AA8" t="inlineStr"/>
-      <c r="AB8" t="inlineStr"/>
+      <c r="Z8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1197,15 +1165,13 @@
       <c r="U9" t="inlineStr"/>
       <c r="V9" t="inlineStr"/>
       <c r="W9" t="inlineStr"/>
-      <c r="X9" t="inlineStr"/>
+      <c r="X9" t="n">
+        <v>15.95</v>
+      </c>
       <c r="Y9" t="n">
-        <v>15.95</v>
-      </c>
-      <c r="Z9" t="n">
         <v>5.033333333333333</v>
       </c>
-      <c r="AA9" t="inlineStr"/>
-      <c r="AB9" t="inlineStr"/>
+      <c r="Z9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1281,22 +1247,16 @@
         <v>0.02903155302235026</v>
       </c>
       <c r="W10" t="n">
-        <v>1.257413181978043</v>
+        <v>130</v>
       </c>
       <c r="X10" t="n">
-        <v>130</v>
+        <v>11.76</v>
       </c>
       <c r="Y10" t="n">
-        <v>11.76</v>
+        <v>5.719074074074074</v>
       </c>
       <c r="Z10" t="n">
-        <v>5.719074074074074</v>
-      </c>
-      <c r="AA10" t="n">
         <v>59286.35242371303</v>
-      </c>
-      <c r="AB10" t="n">
-        <v>1.02164821035716</v>
       </c>
     </row>
     <row r="11">
@@ -1362,20 +1322,18 @@
       <c r="T11" t="inlineStr"/>
       <c r="U11" t="inlineStr"/>
       <c r="V11" t="inlineStr"/>
-      <c r="W11" t="inlineStr"/>
+      <c r="W11" t="n">
+        <v>184</v>
+      </c>
       <c r="X11" t="n">
-        <v>184</v>
+        <v>11.76</v>
       </c>
       <c r="Y11" t="n">
-        <v>11.76</v>
+        <v>11.62518188580831</v>
       </c>
       <c r="Z11" t="n">
-        <v>11.62518188580831</v>
-      </c>
-      <c r="AA11" t="n">
         <v>66644.42727505849</v>
       </c>
-      <c r="AB11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1451,22 +1409,16 @@
         <v>0.01953613012857874</v>
       </c>
       <c r="W12" t="n">
-        <v>0.847484724302772</v>
+        <v>193</v>
       </c>
       <c r="X12" t="n">
-        <v>193</v>
+        <v>11.76</v>
       </c>
       <c r="Y12" t="n">
-        <v>11.76</v>
+        <v>10.96088452380952</v>
       </c>
       <c r="Z12" t="n">
-        <v>10.96088452380952</v>
-      </c>
-      <c r="AA12" t="n">
         <v>62723.71050748076</v>
-      </c>
-      <c r="AB12" t="n">
-        <v>0.6815189657934791</v>
       </c>
     </row>
     <row r="13">
@@ -1543,22 +1495,16 @@
         <v>0.02463412059593207</v>
       </c>
       <c r="W13" t="n">
-        <v>0.9966162976897276</v>
+        <v>198</v>
       </c>
       <c r="X13" t="n">
-        <v>198</v>
+        <v>11.76</v>
       </c>
       <c r="Y13" t="n">
-        <v>11.76</v>
+        <v>5.427586206896552</v>
       </c>
       <c r="Z13" t="n">
-        <v>5.427586206896552</v>
-      </c>
-      <c r="AA13" t="n">
         <v>63904.1570481465</v>
-      </c>
-      <c r="AB13" t="n">
-        <v>0.8969546679207548</v>
       </c>
     </row>
     <row r="14">
@@ -1635,22 +1581,16 @@
         <v>0.01696073283616569</v>
       </c>
       <c r="W14" t="n">
-        <v>1.223822284874495</v>
+        <v>265</v>
       </c>
       <c r="X14" t="n">
-        <v>265</v>
+        <v>17.38</v>
       </c>
       <c r="Y14" t="n">
-        <v>17.38</v>
+        <v>5.039999999999999</v>
       </c>
       <c r="Z14" t="n">
-        <v>5.039999999999999</v>
-      </c>
-      <c r="AA14" t="n">
         <v>136739.3352384174</v>
-      </c>
-      <c r="AB14" t="n">
-        <v>0.7988002598318749</v>
       </c>
     </row>
     <row r="15">
@@ -1727,22 +1667,16 @@
         <v>0.01778316284633774</v>
       </c>
       <c r="W15" t="n">
-        <v>1.202775856096727</v>
+        <v>292</v>
       </c>
       <c r="X15" t="n">
-        <v>292</v>
+        <v>16.83</v>
       </c>
       <c r="Y15" t="n">
-        <v>16.83</v>
+        <v>5.050909090909091</v>
       </c>
       <c r="Z15" t="n">
-        <v>5.050909090909091</v>
-      </c>
-      <c r="AA15" t="n">
         <v>127636.338025989</v>
-      </c>
-      <c r="AB15" t="n">
-        <v>0.7982057954096462</v>
       </c>
     </row>
     <row r="16">
@@ -1789,17 +1723,11 @@
       <c r="U16" t="inlineStr"/>
       <c r="V16" t="inlineStr"/>
       <c r="W16" t="n">
-        <v>0.9752558287908442</v>
-      </c>
-      <c r="X16" t="n">
         <v>280</v>
       </c>
+      <c r="X16" t="inlineStr"/>
       <c r="Y16" t="inlineStr"/>
       <c r="Z16" t="inlineStr"/>
-      <c r="AA16" t="inlineStr"/>
-      <c r="AB16" t="n">
-        <v>0.593633982742253</v>
-      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1875,22 +1803,16 @@
         <v>0.01390384055552749</v>
       </c>
       <c r="W17" t="n">
-        <v>1.053476790935672</v>
+        <v>304</v>
       </c>
       <c r="X17" t="n">
-        <v>304</v>
+        <v>17.05</v>
       </c>
       <c r="Y17" t="n">
-        <v>17.05</v>
+        <v>9.151666666666667</v>
       </c>
       <c r="Z17" t="n">
-        <v>9.151666666666667</v>
-      </c>
-      <c r="AA17" t="n">
         <v>145592.1614376467</v>
-      </c>
-      <c r="AB17" t="n">
-        <v>0.7278566919191916</v>
       </c>
     </row>
     <row r="18">
@@ -1955,22 +1877,16 @@
       <c r="U18" t="inlineStr"/>
       <c r="V18" t="inlineStr"/>
       <c r="W18" t="n">
-        <v>1.517621832235924</v>
+        <v>112</v>
       </c>
       <c r="X18" t="n">
-        <v>112</v>
+        <v>9.039999999999999</v>
       </c>
       <c r="Y18" t="n">
-        <v>9.039999999999999</v>
+        <v>4.605</v>
       </c>
       <c r="Z18" t="n">
-        <v>4.605</v>
-      </c>
-      <c r="AA18" t="n">
         <v>56746.0021118581</v>
-      </c>
-      <c r="AB18" t="n">
-        <v>1.268460038883757</v>
       </c>
     </row>
     <row r="19">
@@ -2026,20 +1942,18 @@
       <c r="T19" t="inlineStr"/>
       <c r="U19" t="inlineStr"/>
       <c r="V19" t="inlineStr"/>
-      <c r="W19" t="inlineStr"/>
+      <c r="W19" t="n">
+        <v>113</v>
+      </c>
       <c r="X19" t="n">
-        <v>113</v>
+        <v>10.44</v>
       </c>
       <c r="Y19" t="n">
-        <v>10.44</v>
+        <v>1.153636363636364</v>
       </c>
       <c r="Z19" t="n">
-        <v>1.153636363636364</v>
-      </c>
-      <c r="AA19" t="n">
         <v>64129.64176091191</v>
       </c>
-      <c r="AB19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -2115,22 +2029,16 @@
         <v>0.02196026262569532</v>
       </c>
       <c r="W20" t="n">
-        <v>1.206455180923881</v>
+        <v>128</v>
       </c>
       <c r="X20" t="n">
-        <v>128</v>
+        <v>12.57</v>
       </c>
       <c r="Y20" t="n">
-        <v>12.57</v>
+        <v>5.227987421383648</v>
       </c>
       <c r="Z20" t="n">
-        <v>5.227987421383648</v>
-      </c>
-      <c r="AA20" t="n">
         <v>52735.91179498754</v>
-      </c>
-      <c r="AB20" t="n">
-        <v>1.036417873545348</v>
       </c>
     </row>
     <row r="21">
@@ -2201,15 +2109,13 @@
         <v>0.02827116541266036</v>
       </c>
       <c r="W21" t="inlineStr"/>
-      <c r="X21" t="inlineStr"/>
+      <c r="X21" t="n">
+        <v>12.83</v>
+      </c>
       <c r="Y21" t="n">
-        <v>12.83</v>
-      </c>
-      <c r="Z21" t="n">
         <v>1.4</v>
       </c>
-      <c r="AA21" t="inlineStr"/>
-      <c r="AB21" t="inlineStr"/>
+      <c r="Z21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -2281,15 +2187,13 @@
         <v>0.02214407354403367</v>
       </c>
       <c r="W22" t="inlineStr"/>
-      <c r="X22" t="inlineStr"/>
+      <c r="X22" t="n">
+        <v>12.55</v>
+      </c>
       <c r="Y22" t="n">
-        <v>12.55</v>
-      </c>
-      <c r="Z22" t="n">
         <v>1.4</v>
       </c>
-      <c r="AA22" t="inlineStr"/>
-      <c r="AB22" t="inlineStr"/>
+      <c r="Z22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -2354,20 +2258,18 @@
       <c r="T23" t="inlineStr"/>
       <c r="U23" t="inlineStr"/>
       <c r="V23" t="inlineStr"/>
-      <c r="W23" t="inlineStr"/>
+      <c r="W23" t="n">
+        <v>131</v>
+      </c>
       <c r="X23" t="n">
-        <v>131</v>
+        <v>11.13</v>
       </c>
       <c r="Y23" t="n">
-        <v>11.13</v>
+        <v>5.1</v>
       </c>
       <c r="Z23" t="n">
-        <v>5.1</v>
-      </c>
-      <c r="AA23" t="n">
         <v>53907.19238070866</v>
       </c>
-      <c r="AB23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -2443,22 +2345,16 @@
         <v>0.02935783987608479</v>
       </c>
       <c r="W24" t="n">
-        <v>1.475470707385693</v>
+        <v>113</v>
       </c>
       <c r="X24" t="n">
-        <v>113</v>
+        <v>12.41</v>
       </c>
       <c r="Y24" t="n">
-        <v>12.41</v>
+        <v>5.351851851851851</v>
       </c>
       <c r="Z24" t="n">
-        <v>5.351851851851851</v>
-      </c>
-      <c r="AA24" t="n">
         <v>54112.65556012069</v>
-      </c>
-      <c r="AB24" t="n">
-        <v>1.149849585755747</v>
       </c>
     </row>
     <row r="25">
@@ -2521,22 +2417,16 @@
       <c r="U25" t="inlineStr"/>
       <c r="V25" t="inlineStr"/>
       <c r="W25" t="n">
-        <v>1.48783112190594</v>
+        <v>186</v>
       </c>
       <c r="X25" t="n">
-        <v>186</v>
+        <v>15.85</v>
       </c>
       <c r="Y25" t="n">
-        <v>15.85</v>
+        <v>5.024999999999999</v>
       </c>
       <c r="Z25" t="n">
-        <v>5.024999999999999</v>
-      </c>
-      <c r="AA25" t="n">
         <v>102716.4593636025</v>
-      </c>
-      <c r="AB25" t="n">
-        <v>0.9542640988776029</v>
       </c>
     </row>
     <row r="26">
@@ -2601,20 +2491,14 @@
       <c r="U26" t="inlineStr"/>
       <c r="V26" t="inlineStr"/>
       <c r="W26" t="n">
-        <v>1.175359044474089</v>
-      </c>
-      <c r="X26" t="n">
         <v>226</v>
       </c>
-      <c r="Y26" t="inlineStr"/>
+      <c r="X26" t="inlineStr"/>
+      <c r="Y26" t="n">
+        <v>9.109334158730158</v>
+      </c>
       <c r="Z26" t="n">
-        <v>9.109334158730158</v>
-      </c>
-      <c r="AA26" t="n">
         <v>116758.9964281686</v>
-      </c>
-      <c r="AB26" t="n">
-        <v>0.6971946038087771</v>
       </c>
     </row>
     <row r="27">
@@ -2679,20 +2563,14 @@
       <c r="U27" t="inlineStr"/>
       <c r="V27" t="inlineStr"/>
       <c r="W27" t="n">
-        <v>1.14505117943573</v>
-      </c>
-      <c r="X27" t="n">
         <v>266</v>
       </c>
-      <c r="Y27" t="inlineStr"/>
+      <c r="X27" t="inlineStr"/>
+      <c r="Y27" t="n">
+        <v>8.926964901960785</v>
+      </c>
       <c r="Z27" t="n">
-        <v>8.926964901960785</v>
-      </c>
-      <c r="AA27" t="n">
         <v>123416.9352806504</v>
-      </c>
-      <c r="AB27" t="n">
-        <v>0.7251990803092957</v>
       </c>
     </row>
     <row r="28">
@@ -2754,20 +2632,18 @@
       <c r="T28" t="inlineStr"/>
       <c r="U28" t="inlineStr"/>
       <c r="V28" t="inlineStr"/>
-      <c r="W28" t="inlineStr"/>
+      <c r="W28" t="n">
+        <v>108</v>
+      </c>
       <c r="X28" t="n">
-        <v>108</v>
+        <v>11.28</v>
       </c>
       <c r="Y28" t="n">
-        <v>11.28</v>
+        <v>1.045</v>
       </c>
       <c r="Z28" t="n">
-        <v>1.045</v>
-      </c>
-      <c r="AA28" t="n">
         <v>59227.28086090866</v>
       </c>
-      <c r="AB28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -2843,22 +2719,16 @@
         <v>0.02324392599335197</v>
       </c>
       <c r="W29" t="n">
-        <v>1.025375544030074</v>
+        <v>163</v>
       </c>
       <c r="X29" t="n">
-        <v>163</v>
+        <v>12.57</v>
       </c>
       <c r="Y29" t="n">
-        <v>12.57</v>
+        <v>5.132291666666666</v>
       </c>
       <c r="Z29" t="n">
-        <v>5.132291666666666</v>
-      </c>
-      <c r="AA29" t="n">
         <v>54584.23347610084</v>
-      </c>
-      <c r="AB29" t="n">
-        <v>0.8843185908830796</v>
       </c>
     </row>
     <row r="30">
@@ -2935,22 +2805,16 @@
         <v>0.02326096513409742</v>
       </c>
       <c r="W30" t="n">
-        <v>1.033776048227667</v>
+        <v>175</v>
       </c>
       <c r="X30" t="n">
-        <v>175</v>
+        <v>12.57</v>
       </c>
       <c r="Y30" t="n">
-        <v>12.57</v>
+        <v>5.144374999999999</v>
       </c>
       <c r="Z30" t="n">
-        <v>5.144374999999999</v>
-      </c>
-      <c r="AA30" t="n">
         <v>64729.8892720201</v>
-      </c>
-      <c r="AB30" t="n">
-        <v>0.9572000446552472</v>
       </c>
     </row>
     <row r="31">
@@ -3027,22 +2891,16 @@
         <v>0.03112426042970285</v>
       </c>
       <c r="W31" t="n">
-        <v>1.127427684674653</v>
+        <v>179</v>
       </c>
       <c r="X31" t="n">
-        <v>179</v>
+        <v>12.57</v>
       </c>
       <c r="Y31" t="n">
-        <v>12.57</v>
+        <v>5.1359375</v>
       </c>
       <c r="Z31" t="n">
-        <v>5.1359375</v>
-      </c>
-      <c r="AA31" t="n">
         <v>55164.22753360885</v>
-      </c>
-      <c r="AB31" t="n">
-        <v>0.9173161616216495</v>
       </c>
     </row>
     <row r="32">
@@ -3119,22 +2977,16 @@
         <v>0.01880167355940041</v>
       </c>
       <c r="W32" t="n">
-        <v>1.607596036522946</v>
+        <v>405</v>
       </c>
       <c r="X32" t="n">
-        <v>405</v>
+        <v>19.3</v>
       </c>
       <c r="Y32" t="n">
-        <v>19.3</v>
+        <v>5.01875</v>
       </c>
       <c r="Z32" t="n">
-        <v>5.01875</v>
-      </c>
-      <c r="AA32" t="n">
         <v>235054.4768945164</v>
-      </c>
-      <c r="AB32" t="n">
-        <v>1.479719079072257</v>
       </c>
     </row>
     <row r="33">
@@ -3198,20 +3050,18 @@
       <c r="T33" t="inlineStr"/>
       <c r="U33" t="inlineStr"/>
       <c r="V33" t="inlineStr"/>
-      <c r="W33" t="inlineStr"/>
+      <c r="W33" t="n">
+        <v>248</v>
+      </c>
       <c r="X33" t="n">
-        <v>248</v>
+        <v>20.2</v>
       </c>
       <c r="Y33" t="n">
-        <v>20.2</v>
+        <v>4.6275</v>
       </c>
       <c r="Z33" t="n">
-        <v>4.6275</v>
-      </c>
-      <c r="AA33" t="n">
         <v>199548.9932938909</v>
       </c>
-      <c r="AB33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -3273,22 +3123,16 @@
       <c r="U34" t="inlineStr"/>
       <c r="V34" t="inlineStr"/>
       <c r="W34" t="n">
-        <v>1.174656786481714</v>
+        <v>227</v>
       </c>
       <c r="X34" t="n">
-        <v>227</v>
+        <v>13.6</v>
       </c>
       <c r="Y34" t="n">
-        <v>13.6</v>
+        <v>4.743</v>
       </c>
       <c r="Z34" t="n">
-        <v>4.743</v>
-      </c>
-      <c r="AA34" t="n">
         <v>85293.06457440818</v>
-      </c>
-      <c r="AB34" t="n">
-        <v>0.9038884424791493</v>
       </c>
     </row>
     <row r="35">
@@ -3363,22 +3207,16 @@
         <v>0.03093550516493822</v>
       </c>
       <c r="W35" t="n">
-        <v>1.305531264304784</v>
+        <v>249</v>
       </c>
       <c r="X35" t="n">
-        <v>249</v>
+        <v>16.8</v>
       </c>
       <c r="Y35" t="n">
-        <v>16.8</v>
+        <v>5.1</v>
       </c>
       <c r="Z35" t="n">
-        <v>5.1</v>
-      </c>
-      <c r="AA35" t="n">
         <v>115566.7293916298</v>
-      </c>
-      <c r="AB35" t="n">
-        <v>0.8668727594983766</v>
       </c>
     </row>
     <row r="36">
@@ -3453,22 +3291,16 @@
         <v>0.01332857535578807</v>
       </c>
       <c r="W36" t="n">
-        <v>1.362634274000017</v>
+        <v>329</v>
       </c>
       <c r="X36" t="n">
-        <v>329</v>
+        <v>18.5</v>
       </c>
       <c r="Y36" t="n">
-        <v>18.5</v>
+        <v>6.571666666666667</v>
       </c>
       <c r="Z36" t="n">
-        <v>6.571666666666667</v>
-      </c>
-      <c r="AA36" t="n">
         <v>169077.3922160371</v>
-      </c>
-      <c r="AB36" t="n">
-        <v>0.815103047538192</v>
       </c>
     </row>
     <row r="37">
@@ -3533,20 +3365,14 @@
       <c r="U37" t="inlineStr"/>
       <c r="V37" t="inlineStr"/>
       <c r="W37" t="n">
-        <v>0.9950608429392854</v>
-      </c>
-      <c r="X37" t="n">
         <v>318</v>
       </c>
-      <c r="Y37" t="inlineStr"/>
+      <c r="X37" t="inlineStr"/>
+      <c r="Y37" t="n">
+        <v>8.697134444444444</v>
+      </c>
       <c r="Z37" t="n">
-        <v>8.697134444444444</v>
-      </c>
-      <c r="AA37" t="n">
         <v>124313.2037511073</v>
-      </c>
-      <c r="AB37" t="n">
-        <v>0.7191576092152108</v>
       </c>
     </row>
     <row r="38">
@@ -3619,15 +3445,13 @@
         <v>0.0156671522231543</v>
       </c>
       <c r="W38" t="inlineStr"/>
-      <c r="X38" t="inlineStr"/>
+      <c r="X38" t="n">
+        <v>11.79</v>
+      </c>
       <c r="Y38" t="n">
-        <v>11.79</v>
-      </c>
-      <c r="Z38" t="n">
         <v>1.4</v>
       </c>
-      <c r="AA38" t="inlineStr"/>
-      <c r="AB38" t="inlineStr"/>
+      <c r="Z38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -3682,20 +3506,18 @@
       <c r="T39" t="inlineStr"/>
       <c r="U39" t="inlineStr"/>
       <c r="V39" t="inlineStr"/>
-      <c r="W39" t="inlineStr"/>
+      <c r="W39" t="n">
+        <v>150</v>
+      </c>
       <c r="X39" t="n">
-        <v>150</v>
+        <v>10.65</v>
       </c>
       <c r="Y39" t="n">
-        <v>10.65</v>
+        <v>1.026923076923077</v>
       </c>
       <c r="Z39" t="n">
-        <v>1.026923076923077</v>
-      </c>
-      <c r="AA39" t="n">
         <v>73527.22856566517</v>
       </c>
-      <c r="AB39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -3771,22 +3593,16 @@
         <v>0.01734715984225846</v>
       </c>
       <c r="W40" t="n">
-        <v>0.8353390780716035</v>
+        <v>171</v>
       </c>
       <c r="X40" t="n">
-        <v>171</v>
+        <v>12.29</v>
       </c>
       <c r="Y40" t="n">
-        <v>12.29</v>
+        <v>8.435416666666667</v>
       </c>
       <c r="Z40" t="n">
-        <v>8.435416666666667</v>
-      </c>
-      <c r="AA40" t="n">
         <v>55505.42800502713</v>
-      </c>
-      <c r="AB40" t="n">
-        <v>0.6802046778583057</v>
       </c>
     </row>
     <row r="41">
@@ -3861,22 +3677,16 @@
         <v>0.01784314606759582</v>
       </c>
       <c r="W41" t="n">
-        <v>0.8795860416327073</v>
+        <v>178</v>
       </c>
       <c r="X41" t="n">
-        <v>178</v>
+        <v>12.29</v>
       </c>
       <c r="Y41" t="n">
-        <v>12.29</v>
+        <v>8.447222222222223</v>
       </c>
       <c r="Z41" t="n">
-        <v>8.447222222222223</v>
-      </c>
-      <c r="AA41" t="n">
         <v>49433.32369637736</v>
-      </c>
-      <c r="AB41" t="n">
-        <v>0.7116650700482813</v>
       </c>
     </row>
     <row r="42">
@@ -3949,22 +3759,16 @@
         <v>0.0237282131256938</v>
       </c>
       <c r="W42" t="n">
-        <v>1.848998853040951</v>
+        <v>109</v>
       </c>
       <c r="X42" t="n">
-        <v>109</v>
+        <v>11.28</v>
       </c>
       <c r="Y42" t="n">
-        <v>11.28</v>
+        <v>1.045</v>
       </c>
       <c r="Z42" t="n">
-        <v>1.045</v>
-      </c>
-      <c r="AA42" t="n">
         <v>52000.1441749647</v>
-      </c>
-      <c r="AB42" t="n">
-        <v>1.550314422934336</v>
       </c>
     </row>
     <row r="43">
@@ -4041,22 +3845,16 @@
         <v>0.03370308000006633</v>
       </c>
       <c r="W43" t="n">
-        <v>1.300332435026857</v>
+        <v>143</v>
       </c>
       <c r="X43" t="n">
-        <v>143</v>
+        <v>11.13</v>
       </c>
       <c r="Y43" t="n">
-        <v>11.13</v>
+        <v>5.1</v>
       </c>
       <c r="Z43" t="n">
-        <v>5.1</v>
-      </c>
-      <c r="AA43" t="n">
         <v>55491.06311528273</v>
-      </c>
-      <c r="AB43" t="n">
-        <v>0.9890826500470241</v>
       </c>
     </row>
     <row r="44">
@@ -4133,22 +3931,16 @@
         <v>0.02812387631907114</v>
       </c>
       <c r="W44" t="n">
-        <v>1.96228034370375</v>
+        <v>391</v>
       </c>
       <c r="X44" t="n">
-        <v>391</v>
+        <v>18.14285714285714</v>
       </c>
       <c r="Y44" t="n">
-        <v>18.14285714285714</v>
+        <v>4.620535714285714</v>
       </c>
       <c r="Z44" t="n">
-        <v>4.620535714285714</v>
-      </c>
-      <c r="AA44" t="n">
         <v>248451.1329570788</v>
-      </c>
-      <c r="AB44" t="n">
-        <v>1.395002935251211</v>
       </c>
     </row>
     <row r="45">
@@ -4223,22 +4015,16 @@
         <v>0.01684179534228456</v>
       </c>
       <c r="W45" t="n">
-        <v>1.567817459973697</v>
+        <v>386</v>
       </c>
       <c r="X45" t="n">
-        <v>386</v>
+        <v>19.4</v>
       </c>
       <c r="Y45" t="n">
-        <v>19.4</v>
+        <v>4.54</v>
       </c>
       <c r="Z45" t="n">
-        <v>4.54</v>
-      </c>
-      <c r="AA45" t="n">
         <v>260013.3369929212</v>
-      </c>
-      <c r="AB45" t="n">
-        <v>1.10032279918154</v>
       </c>
     </row>
     <row r="46">
@@ -4301,22 +4087,16 @@
       <c r="U46" t="inlineStr"/>
       <c r="V46" t="inlineStr"/>
       <c r="W46" t="n">
-        <v>1.30972191201682</v>
+        <v>186</v>
       </c>
       <c r="X46" t="n">
-        <v>186</v>
+        <v>13.74</v>
       </c>
       <c r="Y46" t="n">
-        <v>13.74</v>
+        <v>4.7025</v>
       </c>
       <c r="Z46" t="n">
-        <v>4.7025</v>
-      </c>
-      <c r="AA46" t="n">
         <v>73284.27730044253</v>
-      </c>
-      <c r="AB46" t="n">
-        <v>1.01928148801309</v>
       </c>
     </row>
     <row r="47">
@@ -4379,22 +4159,16 @@
       <c r="U47" t="inlineStr"/>
       <c r="V47" t="inlineStr"/>
       <c r="W47" t="n">
-        <v>1.322512080118051</v>
+        <v>228</v>
       </c>
       <c r="X47" t="n">
-        <v>228</v>
+        <v>15.85</v>
       </c>
       <c r="Y47" t="n">
-        <v>15.85</v>
+        <v>4.846153846153846</v>
       </c>
       <c r="Z47" t="n">
-        <v>4.846153846153846</v>
-      </c>
-      <c r="AA47" t="n">
         <v>105769.5470134647</v>
-      </c>
-      <c r="AB47" t="n">
-        <v>0.8590676759741186</v>
       </c>
     </row>
     <row r="48">
@@ -4469,22 +4243,16 @@
         <v>0.01364819352291468</v>
       </c>
       <c r="W48" t="n">
-        <v>1.540685556401292</v>
+        <v>273</v>
       </c>
       <c r="X48" t="n">
-        <v>273</v>
+        <v>18.41666666666667</v>
       </c>
       <c r="Y48" t="n">
-        <v>18.41666666666667</v>
+        <v>7.264416666666667</v>
       </c>
       <c r="Z48" t="n">
-        <v>7.264416666666667</v>
-      </c>
-      <c r="AA48" t="n">
         <v>166950.6603020956</v>
-      </c>
-      <c r="AB48" t="n">
-        <v>0.9559253565853472</v>
       </c>
     </row>
     <row r="49">
@@ -4544,18 +4312,16 @@
       <c r="T49" t="inlineStr"/>
       <c r="U49" t="inlineStr"/>
       <c r="V49" t="inlineStr"/>
-      <c r="W49" t="inlineStr"/>
-      <c r="X49" t="n">
+      <c r="W49" t="n">
         <v>50</v>
       </c>
-      <c r="Y49" t="inlineStr"/>
+      <c r="X49" t="inlineStr"/>
+      <c r="Y49" t="n">
+        <v>6.25</v>
+      </c>
       <c r="Z49" t="n">
-        <v>6.25</v>
-      </c>
-      <c r="AA49" t="n">
         <v>60183.58157575225</v>
       </c>
-      <c r="AB49" t="inlineStr"/>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -4620,20 +4386,18 @@
       <c r="T50" t="inlineStr"/>
       <c r="U50" t="inlineStr"/>
       <c r="V50" t="inlineStr"/>
-      <c r="W50" t="inlineStr"/>
+      <c r="W50" t="n">
+        <v>76</v>
+      </c>
       <c r="X50" t="n">
-        <v>76</v>
+        <v>7.5</v>
       </c>
       <c r="Y50" t="n">
-        <v>7.5</v>
+        <v>5.13</v>
       </c>
       <c r="Z50" t="n">
-        <v>5.13</v>
-      </c>
-      <c r="AA50" t="n">
         <v>53867.34395398862</v>
       </c>
-      <c r="AB50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -4698,98 +4462,72 @@
       <c r="T51" t="inlineStr"/>
       <c r="U51" t="inlineStr"/>
       <c r="V51" t="inlineStr"/>
-      <c r="W51" t="inlineStr"/>
+      <c r="W51" t="n">
+        <v>67</v>
+      </c>
       <c r="X51" t="n">
-        <v>67</v>
+        <v>7.599999999999999</v>
       </c>
       <c r="Y51" t="n">
-        <v>7.599999999999999</v>
+        <v>5.13</v>
       </c>
       <c r="Z51" t="n">
-        <v>5.13</v>
-      </c>
-      <c r="AA51" t="n">
         <v>35311.07862111123</v>
       </c>
-      <c r="AB51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Embraer</t>
+          <t>De Havilland</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Embraer 190</t>
+          <t>Comet 4</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Regional</t>
+          <t>Narrow</t>
         </is>
       </c>
       <c r="D52" t="n">
-        <v>2004</v>
-      </c>
-      <c r="E52" t="n">
-        <v>51843.125</v>
-      </c>
-      <c r="F52" t="n">
-        <v>44140.625</v>
-      </c>
+        <v>1958</v>
+      </c>
+      <c r="E52" t="inlineStr"/>
+      <c r="F52" t="inlineStr"/>
       <c r="G52" t="n">
-        <v>124</v>
-      </c>
-      <c r="H52" t="n">
-        <v>16347.75</v>
-      </c>
+        <v>109</v>
+      </c>
+      <c r="H52" t="inlineStr"/>
       <c r="I52" t="n">
-        <v>16.77016917536357</v>
+        <v>30.62663043478261</v>
       </c>
       <c r="J52" t="n">
-        <v>0.3392881252903102</v>
+        <v>0.1846523950527501</v>
       </c>
       <c r="K52" t="n">
-        <v>1.712372106412916</v>
+        <v>3.451363636363636</v>
       </c>
       <c r="L52" t="n">
-        <v>226.7204301075269</v>
-      </c>
-      <c r="M52" t="inlineStr"/>
-      <c r="N52" t="n">
-        <v>9.754665681149657</v>
-      </c>
-      <c r="O52" t="n">
-        <v>0.04141733060561711</v>
-      </c>
-      <c r="P52" t="n">
-        <v>30.545</v>
-      </c>
-      <c r="Q52" t="n">
-        <v>0.7117598908588553</v>
-      </c>
-      <c r="R52" t="n">
-        <v>0.4763098239510975</v>
-      </c>
+        <v>313.8715596330275</v>
+      </c>
+      <c r="M52" t="n">
+        <v>15.01504580607603</v>
+      </c>
+      <c r="N52" t="inlineStr"/>
+      <c r="O52" t="inlineStr"/>
+      <c r="P52" t="inlineStr"/>
+      <c r="Q52" t="inlineStr"/>
+      <c r="R52" t="inlineStr"/>
       <c r="S52" t="inlineStr"/>
       <c r="T52" t="inlineStr"/>
       <c r="U52" t="inlineStr"/>
       <c r="V52" t="inlineStr"/>
       <c r="W52" t="inlineStr"/>
-      <c r="X52" t="n">
-        <v>99</v>
-      </c>
-      <c r="Y52" t="n">
-        <v>10.605</v>
-      </c>
-      <c r="Z52" t="n">
-        <v>7.026875</v>
-      </c>
-      <c r="AA52" t="n">
-        <v>61088.37579710694</v>
-      </c>
-      <c r="AB52" t="inlineStr"/>
+      <c r="X52" t="inlineStr"/>
+      <c r="Y52" t="inlineStr"/>
+      <c r="Z52" t="inlineStr"/>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -4799,7 +4537,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Embraer-135</t>
+          <t>Embraer 190</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -4808,64 +4546,64 @@
         </is>
       </c>
       <c r="D53" t="n">
-        <v>1999</v>
+        <v>2004</v>
       </c>
       <c r="E53" t="n">
-        <v>21096</v>
+        <v>51843.125</v>
       </c>
       <c r="F53" t="n">
-        <v>15840</v>
+        <v>44140.625</v>
       </c>
       <c r="G53" t="n">
-        <v>37</v>
+        <v>124</v>
       </c>
       <c r="H53" t="n">
-        <v>8216.799999999999</v>
+        <v>16347.75</v>
       </c>
       <c r="I53" t="n">
-        <v>18.16621531661354</v>
+        <v>16.77016917536357</v>
       </c>
       <c r="J53" t="n">
-        <v>0.3113135990720869</v>
-      </c>
-      <c r="K53" t="inlineStr"/>
+        <v>0.3392881252903102</v>
+      </c>
+      <c r="K53" t="n">
+        <v>1.712372106412916</v>
+      </c>
       <c r="L53" t="n">
-        <v>339.1891891891892</v>
+        <v>226.7204301075269</v>
       </c>
       <c r="M53" t="inlineStr"/>
       <c r="N53" t="n">
-        <v>7.846846424384525</v>
+        <v>9.754665681149657</v>
       </c>
       <c r="O53" t="n">
-        <v>0.05070665796303604</v>
+        <v>0.04141733060561711</v>
       </c>
       <c r="P53" t="n">
-        <v>20.04</v>
+        <v>30.545</v>
       </c>
       <c r="Q53" t="n">
-        <v>0.5445136717279478</v>
+        <v>0.7117598908588553</v>
       </c>
       <c r="R53" t="n">
-        <v>0.5717351067638586</v>
+        <v>0.4763098239510975</v>
       </c>
       <c r="S53" t="inlineStr"/>
       <c r="T53" t="inlineStr"/>
       <c r="U53" t="inlineStr"/>
       <c r="V53" t="inlineStr"/>
-      <c r="W53" t="inlineStr"/>
+      <c r="W53" t="n">
+        <v>99</v>
+      </c>
       <c r="X53" t="n">
-        <v>37</v>
+        <v>10.605</v>
       </c>
       <c r="Y53" t="n">
-        <v>6.76</v>
+        <v>7.026875</v>
       </c>
       <c r="Z53" t="n">
-        <v>4.762</v>
-      </c>
-      <c r="AA53" t="n">
-        <v>58122.6644342903</v>
-      </c>
-      <c r="AB53" t="inlineStr"/>
+        <v>61088.37579710694</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -4875,7 +4613,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Embraer-140</t>
+          <t>Embraer-135</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
@@ -4884,46 +4622,72 @@
         </is>
       </c>
       <c r="D54" t="n">
-        <v>2001</v>
-      </c>
-      <c r="E54" t="inlineStr"/>
-      <c r="F54" t="inlineStr"/>
+        <v>1999</v>
+      </c>
+      <c r="E54" t="n">
+        <v>21096</v>
+      </c>
+      <c r="F54" t="n">
+        <v>15840</v>
+      </c>
       <c r="G54" t="n">
-        <v>44</v>
-      </c>
-      <c r="H54" t="inlineStr"/>
-      <c r="I54" t="inlineStr"/>
-      <c r="J54" t="inlineStr"/>
+        <v>37</v>
+      </c>
+      <c r="H54" t="n">
+        <v>8216.799999999999</v>
+      </c>
+      <c r="I54" t="n">
+        <v>18.16621531661354</v>
+      </c>
+      <c r="J54" t="n">
+        <v>0.3113135990720869</v>
+      </c>
       <c r="K54" t="inlineStr"/>
       <c r="L54" t="n">
-        <v>268.1818181818182</v>
+        <v>339.1891891891892</v>
       </c>
       <c r="M54" t="inlineStr"/>
-      <c r="N54" t="inlineStr"/>
-      <c r="O54" t="inlineStr"/>
-      <c r="P54" t="inlineStr"/>
-      <c r="Q54" t="inlineStr"/>
-      <c r="R54" t="inlineStr"/>
+      <c r="N54" t="n">
+        <v>7.846846424384525</v>
+      </c>
+      <c r="O54" t="n">
+        <v>0.05070665796303604</v>
+      </c>
+      <c r="P54" t="n">
+        <v>20.04</v>
+      </c>
+      <c r="Q54" t="n">
+        <v>0.5445136717279478</v>
+      </c>
+      <c r="R54" t="n">
+        <v>0.5717351067638586</v>
+      </c>
       <c r="S54" t="inlineStr"/>
       <c r="T54" t="inlineStr"/>
       <c r="U54" t="inlineStr"/>
       <c r="V54" t="inlineStr"/>
-      <c r="W54" t="inlineStr"/>
-      <c r="X54" t="inlineStr"/>
-      <c r="Y54" t="inlineStr"/>
-      <c r="Z54" t="inlineStr"/>
-      <c r="AA54" t="inlineStr"/>
-      <c r="AB54" t="inlineStr"/>
+      <c r="W54" t="n">
+        <v>37</v>
+      </c>
+      <c r="X54" t="n">
+        <v>6.76</v>
+      </c>
+      <c r="Y54" t="n">
+        <v>4.762</v>
+      </c>
+      <c r="Z54" t="n">
+        <v>58122.6644342903</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t xml:space="preserve">Embraer </t>
+          <t>Embraer</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>EMB-120 Brasilia</t>
+          <t>Embraer-140</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
@@ -4932,19 +4696,19 @@
         </is>
       </c>
       <c r="D55" t="n">
-        <v>1985</v>
+        <v>2001</v>
       </c>
       <c r="E55" t="inlineStr"/>
       <c r="F55" t="inlineStr"/>
       <c r="G55" t="n">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="H55" t="inlineStr"/>
       <c r="I55" t="inlineStr"/>
       <c r="J55" t="inlineStr"/>
       <c r="K55" t="inlineStr"/>
       <c r="L55" t="n">
-        <v>252</v>
+        <v>268.1818181818182</v>
       </c>
       <c r="M55" t="inlineStr"/>
       <c r="N55" t="inlineStr"/>
@@ -4960,8 +4724,6 @@
       <c r="X55" t="inlineStr"/>
       <c r="Y55" t="inlineStr"/>
       <c r="Z55" t="inlineStr"/>
-      <c r="AA55" t="inlineStr"/>
-      <c r="AB55" t="inlineStr"/>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -4971,7 +4733,7 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Embraer ERJ-175</t>
+          <t>EMB-120 Brasilia</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
@@ -4980,66 +4742,34 @@
         </is>
       </c>
       <c r="D56" t="n">
-        <v>2005</v>
-      </c>
-      <c r="E56" t="n">
-        <v>37500</v>
-      </c>
-      <c r="F56" t="n">
-        <v>31700</v>
-      </c>
+        <v>1985</v>
+      </c>
+      <c r="E56" t="inlineStr"/>
+      <c r="F56" t="inlineStr"/>
       <c r="G56" t="n">
-        <v>88</v>
-      </c>
-      <c r="H56" t="n">
-        <v>11625</v>
-      </c>
-      <c r="I56" t="n">
-        <v>18.19340342917936</v>
-      </c>
-      <c r="J56" t="n">
-        <v>0.3108455349745253</v>
-      </c>
-      <c r="K56" t="n">
-        <v>1.431502217381948</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="H56" t="inlineStr"/>
+      <c r="I56" t="inlineStr"/>
+      <c r="J56" t="inlineStr"/>
+      <c r="K56" t="inlineStr"/>
       <c r="L56" t="n">
-        <v>247.8409090909091</v>
+        <v>252</v>
       </c>
       <c r="M56" t="inlineStr"/>
-      <c r="N56" t="n">
-        <v>11.28743811881188</v>
-      </c>
-      <c r="O56" t="n">
-        <v>0.03525045750342684</v>
-      </c>
-      <c r="P56" t="n">
-        <v>28.65</v>
-      </c>
-      <c r="Q56" t="n">
-        <v>0.7278831819159528</v>
-      </c>
-      <c r="R56" t="n">
-        <v>0.4270556565750555</v>
-      </c>
+      <c r="N56" t="inlineStr"/>
+      <c r="O56" t="inlineStr"/>
+      <c r="P56" t="inlineStr"/>
+      <c r="Q56" t="inlineStr"/>
+      <c r="R56" t="inlineStr"/>
       <c r="S56" t="inlineStr"/>
       <c r="T56" t="inlineStr"/>
       <c r="U56" t="inlineStr"/>
       <c r="V56" t="inlineStr"/>
       <c r="W56" t="inlineStr"/>
-      <c r="X56" t="n">
-        <v>75</v>
-      </c>
-      <c r="Y56" t="n">
-        <v>9.82</v>
-      </c>
-      <c r="Z56" t="n">
-        <v>5.13</v>
-      </c>
-      <c r="AA56" t="n">
-        <v>37024.53501579123</v>
-      </c>
-      <c r="AB56" t="inlineStr"/>
+      <c r="X56" t="inlineStr"/>
+      <c r="Y56" t="inlineStr"/>
+      <c r="Z56" t="inlineStr"/>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -5049,7 +4779,7 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Embraer-145</t>
+          <t>Embraer ERJ-175</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
@@ -5058,76 +4788,74 @@
         </is>
       </c>
       <c r="D57" t="n">
-        <v>1996</v>
+        <v>2005</v>
       </c>
       <c r="E57" t="n">
-        <v>20016.66666666667</v>
+        <v>37500</v>
       </c>
       <c r="F57" t="n">
-        <v>17333.33333333333</v>
+        <v>31700</v>
       </c>
       <c r="G57" t="n">
-        <v>50</v>
+        <v>88</v>
       </c>
       <c r="H57" t="n">
-        <v>5528</v>
+        <v>11625</v>
       </c>
       <c r="I57" t="n">
-        <v>18.22195069609804</v>
+        <v>18.19340342917936</v>
       </c>
       <c r="J57" t="n">
-        <v>0.3103601476304506</v>
+        <v>0.3108455349745253</v>
       </c>
       <c r="K57" t="n">
-        <v>2.16826498481953</v>
+        <v>1.431502217381948</v>
       </c>
       <c r="L57" t="n">
-        <v>244.1333333333333</v>
+        <v>247.8409090909091</v>
       </c>
       <c r="M57" t="inlineStr"/>
       <c r="N57" t="n">
-        <v>7.975146541617818</v>
+        <v>11.28743811881188</v>
       </c>
       <c r="O57" t="n">
-        <v>0.04995164617426398</v>
+        <v>0.03525045750342684</v>
       </c>
       <c r="P57" t="n">
-        <v>20.2</v>
+        <v>28.65</v>
       </c>
       <c r="Q57" t="n">
-        <v>0.5862245828175499</v>
+        <v>0.7278831819159528</v>
       </c>
       <c r="R57" t="n">
-        <v>0.5294266580506256</v>
+        <v>0.4270556565750555</v>
       </c>
       <c r="S57" t="inlineStr"/>
       <c r="T57" t="inlineStr"/>
       <c r="U57" t="inlineStr"/>
       <c r="V57" t="inlineStr"/>
-      <c r="W57" t="inlineStr"/>
+      <c r="W57" t="n">
+        <v>75</v>
+      </c>
       <c r="X57" t="n">
-        <v>50</v>
+        <v>9.82</v>
       </c>
       <c r="Y57" t="n">
-        <v>6.75</v>
+        <v>5.13</v>
       </c>
       <c r="Z57" t="n">
-        <v>4.837777777777777</v>
-      </c>
-      <c r="AA57" t="n">
-        <v>49043.17138807395</v>
-      </c>
-      <c r="AB57" t="inlineStr"/>
+        <v>37024.53501579123</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t xml:space="preserve">Fokker </t>
+          <t xml:space="preserve">Embraer </t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Fokker 100</t>
+          <t>Embraer-145</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
@@ -5136,46 +4864,74 @@
         </is>
       </c>
       <c r="D58" t="n">
-        <v>1988</v>
-      </c>
-      <c r="E58" t="inlineStr"/>
-      <c r="F58" t="inlineStr"/>
+        <v>1996</v>
+      </c>
+      <c r="E58" t="n">
+        <v>20016.66666666667</v>
+      </c>
+      <c r="F58" t="n">
+        <v>17333.33333333333</v>
+      </c>
       <c r="G58" t="n">
-        <v>122</v>
-      </c>
-      <c r="H58" t="inlineStr"/>
-      <c r="I58" t="inlineStr"/>
-      <c r="J58" t="inlineStr"/>
-      <c r="K58" t="inlineStr"/>
+        <v>50</v>
+      </c>
+      <c r="H58" t="n">
+        <v>5528</v>
+      </c>
+      <c r="I58" t="n">
+        <v>18.22195069609804</v>
+      </c>
+      <c r="J58" t="n">
+        <v>0.3103601476304506</v>
+      </c>
+      <c r="K58" t="n">
+        <v>2.16826498481953</v>
+      </c>
       <c r="L58" t="n">
-        <v>202.3142076502733</v>
+        <v>244.1333333333333</v>
       </c>
       <c r="M58" t="inlineStr"/>
-      <c r="N58" t="inlineStr"/>
-      <c r="O58" t="inlineStr"/>
-      <c r="P58" t="inlineStr"/>
-      <c r="Q58" t="inlineStr"/>
-      <c r="R58" t="inlineStr"/>
+      <c r="N58" t="n">
+        <v>7.975146541617818</v>
+      </c>
+      <c r="O58" t="n">
+        <v>0.04995164617426398</v>
+      </c>
+      <c r="P58" t="n">
+        <v>20.2</v>
+      </c>
+      <c r="Q58" t="n">
+        <v>0.5862245828175499</v>
+      </c>
+      <c r="R58" t="n">
+        <v>0.5294266580506256</v>
+      </c>
       <c r="S58" t="inlineStr"/>
       <c r="T58" t="inlineStr"/>
       <c r="U58" t="inlineStr"/>
       <c r="V58" t="inlineStr"/>
-      <c r="W58" t="inlineStr"/>
-      <c r="X58" t="inlineStr"/>
-      <c r="Y58" t="inlineStr"/>
-      <c r="Z58" t="inlineStr"/>
-      <c r="AA58" t="inlineStr"/>
-      <c r="AB58" t="inlineStr"/>
+      <c r="W58" t="n">
+        <v>50</v>
+      </c>
+      <c r="X58" t="n">
+        <v>6.75</v>
+      </c>
+      <c r="Y58" t="n">
+        <v>4.837777777777777</v>
+      </c>
+      <c r="Z58" t="n">
+        <v>49043.17138807395</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t xml:space="preserve">Gates Learjet </t>
+          <t xml:space="preserve">Fokker </t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Lear-31/35/36</t>
+          <t>Fokker 100</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
@@ -5184,16 +4940,20 @@
         </is>
       </c>
       <c r="D59" t="n">
-        <v>1974</v>
+        <v>1988</v>
       </c>
       <c r="E59" t="inlineStr"/>
       <c r="F59" t="inlineStr"/>
-      <c r="G59" t="inlineStr"/>
+      <c r="G59" t="n">
+        <v>122</v>
+      </c>
       <c r="H59" t="inlineStr"/>
       <c r="I59" t="inlineStr"/>
       <c r="J59" t="inlineStr"/>
       <c r="K59" t="inlineStr"/>
-      <c r="L59" t="inlineStr"/>
+      <c r="L59" t="n">
+        <v>202.3142076502733</v>
+      </c>
       <c r="M59" t="inlineStr"/>
       <c r="N59" t="inlineStr"/>
       <c r="O59" t="inlineStr"/>
@@ -5208,90 +4968,58 @@
       <c r="X59" t="inlineStr"/>
       <c r="Y59" t="inlineStr"/>
       <c r="Z59" t="inlineStr"/>
-      <c r="AA59" t="inlineStr"/>
-      <c r="AB59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Lockheed</t>
+          <t xml:space="preserve">Gates Learjet </t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>L1011-1/100/200</t>
+          <t>Lear-31/35/36</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>Wide</t>
+          <t>Regional</t>
         </is>
       </c>
       <c r="D60" t="n">
-        <v>1973</v>
-      </c>
-      <c r="E60" t="n">
-        <v>224982</v>
-      </c>
-      <c r="F60" t="n">
-        <v>153314</v>
-      </c>
-      <c r="G60" t="n">
-        <v>400</v>
-      </c>
-      <c r="H60" t="n">
-        <v>120705</v>
-      </c>
-      <c r="I60" t="n">
-        <v>17.5682</v>
-      </c>
-      <c r="J60" t="n">
-        <v>0.3219043875967976</v>
-      </c>
-      <c r="K60" t="n">
-        <v>1.69015679246197</v>
-      </c>
-      <c r="L60" t="n">
-        <v>277.7625</v>
-      </c>
-      <c r="M60" t="n">
-        <v>14.3153</v>
-      </c>
+        <v>1974</v>
+      </c>
+      <c r="E60" t="inlineStr"/>
+      <c r="F60" t="inlineStr"/>
+      <c r="G60" t="inlineStr"/>
+      <c r="H60" t="inlineStr"/>
+      <c r="I60" t="inlineStr"/>
+      <c r="J60" t="inlineStr"/>
+      <c r="K60" t="inlineStr"/>
+      <c r="L60" t="inlineStr"/>
+      <c r="M60" t="inlineStr"/>
       <c r="N60" t="inlineStr"/>
       <c r="O60" t="inlineStr"/>
       <c r="P60" t="inlineStr"/>
-      <c r="Q60" t="n">
-        <v>0.7611246338515383</v>
-      </c>
-      <c r="R60" t="n">
-        <v>0.4229325570082481</v>
-      </c>
+      <c r="Q60" t="inlineStr"/>
+      <c r="R60" t="inlineStr"/>
       <c r="S60" t="inlineStr"/>
       <c r="T60" t="inlineStr"/>
       <c r="U60" t="inlineStr"/>
       <c r="V60" t="inlineStr"/>
       <c r="W60" t="inlineStr"/>
-      <c r="X60" t="n">
-        <v>313</v>
-      </c>
+      <c r="X60" t="inlineStr"/>
       <c r="Y60" t="inlineStr"/>
-      <c r="Z60" t="n">
-        <v>4.54</v>
-      </c>
-      <c r="AA60" t="n">
-        <v>163349.5957069433</v>
-      </c>
-      <c r="AB60" t="inlineStr"/>
+      <c r="Z60" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t xml:space="preserve">Lockheed </t>
+          <t>Lockheed</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>L1011-500</t>
+          <t>L1011-1/100/200</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
@@ -5300,48 +5028,68 @@
         </is>
       </c>
       <c r="D61" t="n">
-        <v>1979</v>
-      </c>
-      <c r="E61" t="inlineStr"/>
-      <c r="F61" t="inlineStr"/>
+        <v>1973</v>
+      </c>
+      <c r="E61" t="n">
+        <v>224982</v>
+      </c>
+      <c r="F61" t="n">
+        <v>153314</v>
+      </c>
       <c r="G61" t="n">
-        <v>330</v>
-      </c>
-      <c r="H61" t="inlineStr"/>
-      <c r="I61" t="inlineStr"/>
-      <c r="J61" t="inlineStr"/>
+        <v>400</v>
+      </c>
+      <c r="H61" t="n">
+        <v>120705</v>
+      </c>
+      <c r="I61" t="n">
+        <v>17.5682</v>
+      </c>
+      <c r="J61" t="n">
+        <v>0.3219043875967976</v>
+      </c>
       <c r="K61" t="n">
-        <v>1.8209</v>
+        <v>1.69015679246197</v>
       </c>
       <c r="L61" t="n">
-        <v>330.0757575757576</v>
-      </c>
-      <c r="M61" t="inlineStr"/>
+        <v>277.7625</v>
+      </c>
+      <c r="M61" t="n">
+        <v>14.3153</v>
+      </c>
       <c r="N61" t="inlineStr"/>
       <c r="O61" t="inlineStr"/>
       <c r="P61" t="inlineStr"/>
-      <c r="Q61" t="inlineStr"/>
-      <c r="R61" t="inlineStr"/>
+      <c r="Q61" t="n">
+        <v>0.7611246338515383</v>
+      </c>
+      <c r="R61" t="n">
+        <v>0.4229325570082481</v>
+      </c>
       <c r="S61" t="inlineStr"/>
       <c r="T61" t="inlineStr"/>
       <c r="U61" t="inlineStr"/>
       <c r="V61" t="inlineStr"/>
-      <c r="W61" t="inlineStr"/>
+      <c r="W61" t="n">
+        <v>313</v>
+      </c>
       <c r="X61" t="inlineStr"/>
-      <c r="Y61" t="inlineStr"/>
-      <c r="Z61" t="inlineStr"/>
-      <c r="AA61" t="inlineStr"/>
-      <c r="AB61" t="inlineStr"/>
+      <c r="Y61" t="n">
+        <v>4.54</v>
+      </c>
+      <c r="Z61" t="n">
+        <v>163349.5957069433</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>McDonnell Douglas</t>
+          <t xml:space="preserve">Lockheed </t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>DC10-30</t>
+          <t>L1011-500</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
@@ -5350,29 +5098,23 @@
         </is>
       </c>
       <c r="D62" t="n">
-        <v>1972</v>
+        <v>1979</v>
       </c>
       <c r="E62" t="inlineStr"/>
       <c r="F62" t="inlineStr"/>
       <c r="G62" t="n">
-        <v>380</v>
+        <v>330</v>
       </c>
       <c r="H62" t="inlineStr"/>
-      <c r="I62" t="n">
-        <v>17.7708</v>
-      </c>
-      <c r="J62" t="n">
-        <v>0.3182344442668905</v>
-      </c>
+      <c r="I62" t="inlineStr"/>
+      <c r="J62" t="inlineStr"/>
       <c r="K62" t="n">
-        <v>1.803152741832779</v>
+        <v>1.8209</v>
       </c>
       <c r="L62" t="n">
-        <v>318.9342105263158</v>
-      </c>
-      <c r="M62" t="n">
-        <v>15.2348</v>
-      </c>
+        <v>330.0757575757576</v>
+      </c>
+      <c r="M62" t="inlineStr"/>
       <c r="N62" t="inlineStr"/>
       <c r="O62" t="inlineStr"/>
       <c r="P62" t="inlineStr"/>
@@ -5383,15 +5125,9 @@
       <c r="U62" t="inlineStr"/>
       <c r="V62" t="inlineStr"/>
       <c r="W62" t="inlineStr"/>
-      <c r="X62" t="n">
-        <v>271</v>
-      </c>
+      <c r="X62" t="inlineStr"/>
       <c r="Y62" t="inlineStr"/>
       <c r="Z62" t="inlineStr"/>
-      <c r="AA62" t="n">
-        <v>176259.1642868837</v>
-      </c>
-      <c r="AB62" t="inlineStr"/>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -5401,7 +5137,7 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>DC10-40</t>
+          <t>DC10-30</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
@@ -5412,61 +5148,43 @@
       <c r="D63" t="n">
         <v>1972</v>
       </c>
-      <c r="E63" t="n">
-        <v>256280</v>
-      </c>
-      <c r="F63" t="n">
-        <v>177355</v>
-      </c>
+      <c r="E63" t="inlineStr"/>
+      <c r="F63" t="inlineStr"/>
       <c r="G63" t="n">
         <v>380</v>
       </c>
-      <c r="H63" t="n">
-        <v>137520</v>
-      </c>
+      <c r="H63" t="inlineStr"/>
       <c r="I63" t="n">
-        <v>17.4331</v>
+        <v>17.7708</v>
       </c>
       <c r="J63" t="n">
-        <v>0.3243990261157257</v>
+        <v>0.3182344442668905</v>
       </c>
       <c r="K63" t="n">
-        <v>1.815799269772046</v>
+        <v>1.803152741832779</v>
       </c>
       <c r="L63" t="n">
-        <v>323.5526315789473</v>
+        <v>318.9342105263158</v>
       </c>
       <c r="M63" t="n">
-        <v>13.9129</v>
+        <v>15.2348</v>
       </c>
       <c r="N63" t="inlineStr"/>
       <c r="O63" t="inlineStr"/>
       <c r="P63" t="inlineStr"/>
-      <c r="Q63" t="n">
-        <v>0.7498489997700178</v>
-      </c>
-      <c r="R63" t="n">
-        <v>0.4326919339257812</v>
-      </c>
+      <c r="Q63" t="inlineStr"/>
+      <c r="R63" t="inlineStr"/>
       <c r="S63" t="inlineStr"/>
       <c r="T63" t="inlineStr"/>
       <c r="U63" t="inlineStr"/>
       <c r="V63" t="inlineStr"/>
       <c r="W63" t="n">
-        <v>1.528879015518656</v>
-      </c>
-      <c r="X63" t="n">
-        <v>292</v>
-      </c>
+        <v>271</v>
+      </c>
+      <c r="X63" t="inlineStr"/>
       <c r="Y63" t="inlineStr"/>
       <c r="Z63" t="n">
-        <v>4.961538461538462</v>
-      </c>
-      <c r="AA63" t="n">
-        <v>176295.7276686124</v>
-      </c>
-      <c r="AB63" t="n">
-        <v>1.174822822451178</v>
+        <v>176259.1642868837</v>
       </c>
     </row>
     <row r="64">
@@ -5477,72 +5195,66 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>DC9-30</t>
+          <t>DC10-40</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>Narrow</t>
+          <t>Wide</t>
         </is>
       </c>
       <c r="D64" t="n">
-        <v>1966</v>
+        <v>1972</v>
       </c>
       <c r="E64" t="n">
-        <v>47627</v>
+        <v>256280</v>
       </c>
       <c r="F64" t="n">
-        <v>39463</v>
+        <v>177355</v>
       </c>
       <c r="G64" t="n">
-        <v>127</v>
+        <v>380</v>
       </c>
       <c r="H64" t="n">
-        <v>13926</v>
+        <v>137520</v>
       </c>
       <c r="I64" t="n">
-        <v>22.4331</v>
+        <v>17.4331</v>
       </c>
       <c r="J64" t="n">
-        <v>0.2520953707770241</v>
+        <v>0.3243990261157257</v>
       </c>
       <c r="K64" t="n">
-        <v>2.396593879999583</v>
+        <v>1.815799269772046</v>
       </c>
       <c r="L64" t="n">
-        <v>203.0629921259843</v>
+        <v>323.5526315789473</v>
       </c>
       <c r="M64" t="n">
-        <v>13.798</v>
+        <v>13.9129</v>
       </c>
       <c r="N64" t="inlineStr"/>
       <c r="O64" t="inlineStr"/>
-      <c r="P64" t="n">
-        <v>28.44</v>
-      </c>
-      <c r="Q64" t="inlineStr"/>
-      <c r="R64" t="inlineStr"/>
+      <c r="P64" t="inlineStr"/>
+      <c r="Q64" t="n">
+        <v>0.7498489997700178</v>
+      </c>
+      <c r="R64" t="n">
+        <v>0.4326919339257812</v>
+      </c>
       <c r="S64" t="inlineStr"/>
       <c r="T64" t="inlineStr"/>
       <c r="U64" t="inlineStr"/>
       <c r="V64" t="inlineStr"/>
       <c r="W64" t="n">
-        <v>2.234576907236709</v>
-      </c>
-      <c r="X64" t="n">
-        <v>101</v>
-      </c>
+        <v>292</v>
+      </c>
+      <c r="X64" t="inlineStr"/>
       <c r="Y64" t="n">
-        <v>8.4</v>
+        <v>4.961538461538462</v>
       </c>
       <c r="Z64" t="n">
-        <v>1.038181818181818</v>
-      </c>
-      <c r="AA64" t="n">
-        <v>50239.33056833609</v>
-      </c>
-      <c r="AB64" t="n">
-        <v>1.777104469534706</v>
+        <v>176295.7276686124</v>
       </c>
     </row>
     <row r="65">
@@ -5553,7 +5265,7 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>DC9-40</t>
+          <t>DC9-30</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
@@ -5562,33 +5274,35 @@
         </is>
       </c>
       <c r="D65" t="n">
-        <v>1968</v>
+        <v>1966</v>
       </c>
       <c r="E65" t="n">
-        <v>51710</v>
+        <v>47627</v>
       </c>
       <c r="F65" t="n">
-        <v>42184</v>
+        <v>39463</v>
       </c>
       <c r="G65" t="n">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H65" t="n">
         <v>13926</v>
       </c>
       <c r="I65" t="n">
-        <v>22.98764963035378</v>
+        <v>22.4331</v>
       </c>
       <c r="J65" t="n">
-        <v>0.2460964991804533</v>
+        <v>0.2520953707770241</v>
       </c>
       <c r="K65" t="n">
-        <v>2.0777</v>
+        <v>2.396593879999583</v>
       </c>
       <c r="L65" t="n">
-        <v>217.3515625</v>
-      </c>
-      <c r="M65" t="inlineStr"/>
+        <v>203.0629921259843</v>
+      </c>
+      <c r="M65" t="n">
+        <v>13.798</v>
+      </c>
       <c r="N65" t="inlineStr"/>
       <c r="O65" t="inlineStr"/>
       <c r="P65" t="n">
@@ -5600,16 +5314,18 @@
       <c r="T65" t="inlineStr"/>
       <c r="U65" t="inlineStr"/>
       <c r="V65" t="inlineStr"/>
-      <c r="W65" t="inlineStr"/>
-      <c r="X65" t="inlineStr"/>
+      <c r="W65" t="n">
+        <v>101</v>
+      </c>
+      <c r="X65" t="n">
+        <v>8.4</v>
+      </c>
       <c r="Y65" t="n">
-        <v>8.5</v>
+        <v>1.038181818181818</v>
       </c>
       <c r="Z65" t="n">
-        <v>1.036428571428571</v>
-      </c>
-      <c r="AA65" t="inlineStr"/>
-      <c r="AB65" t="inlineStr"/>
+        <v>50239.33056833609</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -5619,7 +5335,7 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>DC9-50</t>
+          <t>DC9-40</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
@@ -5628,37 +5344,37 @@
         </is>
       </c>
       <c r="D66" t="n">
-        <v>1976</v>
+        <v>1968</v>
       </c>
       <c r="E66" t="n">
-        <v>54885</v>
+        <v>51710</v>
       </c>
       <c r="F66" t="n">
-        <v>44679</v>
+        <v>42184</v>
       </c>
       <c r="G66" t="n">
-        <v>139</v>
+        <v>128</v>
       </c>
       <c r="H66" t="n">
         <v>13926</v>
       </c>
       <c r="I66" t="n">
-        <v>23.15547775838727</v>
+        <v>22.98764963035378</v>
       </c>
       <c r="J66" t="n">
-        <v>0.2443182490108967</v>
+        <v>0.2460964991804533</v>
       </c>
       <c r="K66" t="n">
-        <v>2.1014</v>
+        <v>2.0777</v>
       </c>
       <c r="L66" t="n">
-        <v>211.0503597122302</v>
+        <v>217.3515625</v>
       </c>
       <c r="M66" t="inlineStr"/>
       <c r="N66" t="inlineStr"/>
       <c r="O66" t="inlineStr"/>
       <c r="P66" t="n">
-        <v>28.45</v>
+        <v>28.44</v>
       </c>
       <c r="Q66" t="inlineStr"/>
       <c r="R66" t="inlineStr"/>
@@ -5667,15 +5383,13 @@
       <c r="U66" t="inlineStr"/>
       <c r="V66" t="inlineStr"/>
       <c r="W66" t="inlineStr"/>
-      <c r="X66" t="inlineStr"/>
+      <c r="X66" t="n">
+        <v>8.5</v>
+      </c>
       <c r="Y66" t="n">
-        <v>8.6</v>
-      </c>
-      <c r="Z66" t="n">
-        <v>1.04375</v>
-      </c>
-      <c r="AA66" t="inlineStr"/>
-      <c r="AB66" t="inlineStr"/>
+        <v>1.036428571428571</v>
+      </c>
+      <c r="Z66" t="inlineStr"/>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -5685,7 +5399,7 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>MD-90</t>
+          <t>DC9-50</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
@@ -5694,68 +5408,52 @@
         </is>
       </c>
       <c r="D67" t="n">
-        <v>1995</v>
+        <v>1976</v>
       </c>
       <c r="E67" t="n">
-        <v>70760</v>
+        <v>54885</v>
       </c>
       <c r="F67" t="n">
-        <v>58967</v>
+        <v>44679</v>
       </c>
       <c r="G67" t="n">
-        <v>167</v>
+        <v>139</v>
       </c>
       <c r="H67" t="n">
-        <v>22104</v>
+        <v>13926</v>
       </c>
       <c r="I67" t="n">
-        <v>16.99770822716683</v>
+        <v>23.15547775838727</v>
       </c>
       <c r="J67" t="n">
-        <v>0.3327206303053079</v>
+        <v>0.2443182490108967</v>
       </c>
       <c r="K67" t="n">
-        <v>1.340189934684793</v>
+        <v>2.1014</v>
       </c>
       <c r="L67" t="n">
-        <v>242.5489021956088</v>
-      </c>
-      <c r="M67" t="n">
-        <v>12.54450404243209</v>
-      </c>
+        <v>211.0503597122302</v>
+      </c>
+      <c r="M67" t="inlineStr"/>
       <c r="N67" t="inlineStr"/>
       <c r="O67" t="inlineStr"/>
       <c r="P67" t="n">
-        <v>32.87</v>
-      </c>
-      <c r="Q67" t="n">
-        <v>0.7458748318947507</v>
-      </c>
-      <c r="R67" t="n">
-        <v>0.4460862698857084</v>
-      </c>
+        <v>28.45</v>
+      </c>
+      <c r="Q67" t="inlineStr"/>
+      <c r="R67" t="inlineStr"/>
       <c r="S67" t="inlineStr"/>
       <c r="T67" t="inlineStr"/>
       <c r="U67" t="inlineStr"/>
       <c r="V67" t="inlineStr"/>
-      <c r="W67" t="n">
-        <v>1.431159306658041</v>
-      </c>
+      <c r="W67" t="inlineStr"/>
       <c r="X67" t="n">
-        <v>148</v>
+        <v>8.6</v>
       </c>
       <c r="Y67" t="n">
-        <v>9.300000000000001</v>
-      </c>
-      <c r="Z67" t="n">
-        <v>4.74</v>
-      </c>
-      <c r="AA67" t="n">
-        <v>63894.06446530207</v>
-      </c>
-      <c r="AB67" t="n">
-        <v>1.268332798714911</v>
-      </c>
+        <v>1.04375</v>
+      </c>
+      <c r="Z67" t="inlineStr"/>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -5765,7 +5463,7 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>MD80/DC9-80</t>
+          <t>MD-90</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
@@ -5774,136 +5472,144 @@
         </is>
       </c>
       <c r="D68" t="n">
-        <v>1980</v>
+        <v>1995</v>
       </c>
       <c r="E68" t="n">
-        <v>66170.71428571429</v>
+        <v>70760</v>
       </c>
       <c r="F68" t="n">
-        <v>54258.33333333334</v>
+        <v>58967</v>
       </c>
       <c r="G68" t="n">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="H68" t="n">
-        <v>22128.57142857143</v>
+        <v>22104</v>
       </c>
       <c r="I68" t="n">
-        <v>20.744</v>
+        <v>16.99770822716683</v>
       </c>
       <c r="J68" t="n">
-        <v>0.2726224769657761</v>
+        <v>0.3327206303053079</v>
       </c>
       <c r="K68" t="n">
-        <v>1.656668854428058</v>
+        <v>1.340189934684793</v>
       </c>
       <c r="L68" t="n">
-        <v>201.4290697674419</v>
+        <v>242.5489021956088</v>
       </c>
       <c r="M68" t="n">
-        <v>13.9129</v>
-      </c>
-      <c r="N68" t="n">
-        <v>9.609283170080145</v>
-      </c>
-      <c r="O68" t="n">
-        <v>0.04140655974928667</v>
-      </c>
+        <v>12.54450404243209</v>
+      </c>
+      <c r="N68" t="inlineStr"/>
+      <c r="O68" t="inlineStr"/>
       <c r="P68" t="n">
-        <v>32.85</v>
-      </c>
-      <c r="Q68" t="inlineStr"/>
-      <c r="R68" t="inlineStr"/>
-      <c r="S68" t="n">
-        <v>0.4818759914491247</v>
-      </c>
-      <c r="T68" t="n">
-        <v>0.04330909613574976</v>
-      </c>
-      <c r="U68" t="n">
-        <v>0.009614788308106073</v>
-      </c>
-      <c r="V68" t="n">
-        <v>0.03369430782764369</v>
-      </c>
+        <v>32.87</v>
+      </c>
+      <c r="Q68" t="n">
+        <v>0.7458748318947507</v>
+      </c>
+      <c r="R68" t="n">
+        <v>0.4460862698857084</v>
+      </c>
+      <c r="S68" t="inlineStr"/>
+      <c r="T68" t="inlineStr"/>
+      <c r="U68" t="inlineStr"/>
+      <c r="V68" t="inlineStr"/>
       <c r="W68" t="n">
-        <v>1.727304523520158</v>
+        <v>148</v>
       </c>
       <c r="X68" t="n">
-        <v>141</v>
+        <v>9.300000000000001</v>
       </c>
       <c r="Y68" t="n">
-        <v>9</v>
+        <v>4.74</v>
       </c>
       <c r="Z68" t="n">
-        <v>1.725714285714286</v>
-      </c>
-      <c r="AA68" t="n">
-        <v>58224.1917224561</v>
-      </c>
-      <c r="AB68" t="n">
-        <v>1.41598801056013</v>
+        <v>63894.06446530207</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t xml:space="preserve">McDonnell Douglas </t>
+          <t>McDonnell Douglas</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>DC10-10</t>
+          <t>MD80/DC9-80</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>Wide</t>
+          <t>Narrow</t>
         </is>
       </c>
       <c r="D69" t="n">
-        <v>1970</v>
-      </c>
-      <c r="E69" t="inlineStr"/>
-      <c r="F69" t="inlineStr"/>
+        <v>1980</v>
+      </c>
+      <c r="E69" t="n">
+        <v>66170.71428571429</v>
+      </c>
+      <c r="F69" t="n">
+        <v>54258.33333333334</v>
+      </c>
       <c r="G69" t="n">
-        <v>380</v>
-      </c>
-      <c r="H69" t="inlineStr"/>
+        <v>172</v>
+      </c>
+      <c r="H69" t="n">
+        <v>22128.57142857143</v>
+      </c>
       <c r="I69" t="n">
-        <v>17.0953</v>
+        <v>20.744</v>
       </c>
       <c r="J69" t="n">
-        <v>0.3308090915150982</v>
+        <v>0.2726224769657761</v>
       </c>
       <c r="K69" t="n">
-        <v>1.665838405572881</v>
+        <v>1.656668854428058</v>
       </c>
       <c r="L69" t="n">
-        <v>286.6842105263158</v>
+        <v>201.4290697674419</v>
       </c>
       <c r="M69" t="n">
-        <v>14.2003</v>
-      </c>
-      <c r="N69" t="inlineStr"/>
-      <c r="O69" t="inlineStr"/>
-      <c r="P69" t="inlineStr"/>
+        <v>13.9129</v>
+      </c>
+      <c r="N69" t="n">
+        <v>9.609283170080145</v>
+      </c>
+      <c r="O69" t="n">
+        <v>0.04140655974928667</v>
+      </c>
+      <c r="P69" t="n">
+        <v>32.85</v>
+      </c>
       <c r="Q69" t="inlineStr"/>
       <c r="R69" t="inlineStr"/>
-      <c r="S69" t="inlineStr"/>
-      <c r="T69" t="inlineStr"/>
-      <c r="U69" t="inlineStr"/>
-      <c r="V69" t="inlineStr"/>
-      <c r="W69" t="inlineStr"/>
+      <c r="S69" t="n">
+        <v>0.4818759914491247</v>
+      </c>
+      <c r="T69" t="n">
+        <v>0.04330909613574976</v>
+      </c>
+      <c r="U69" t="n">
+        <v>0.009614788308106073</v>
+      </c>
+      <c r="V69" t="n">
+        <v>0.03369430782764369</v>
+      </c>
+      <c r="W69" t="n">
+        <v>141</v>
+      </c>
       <c r="X69" t="n">
-        <v>284</v>
-      </c>
-      <c r="Y69" t="inlineStr"/>
-      <c r="Z69" t="inlineStr"/>
-      <c r="AA69" t="n">
-        <v>169567.8746222493</v>
-      </c>
-      <c r="AB69" t="inlineStr"/>
+        <v>9</v>
+      </c>
+      <c r="Y69" t="n">
+        <v>1.725714285714286</v>
+      </c>
+      <c r="Z69" t="n">
+        <v>58224.1917224561</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -5913,63 +5619,55 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>DC9-10</t>
+          <t>DC10-10</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>Narrow</t>
+          <t>Wide</t>
         </is>
       </c>
       <c r="D70" t="n">
-        <v>1965</v>
-      </c>
-      <c r="E70" t="n">
-        <v>41141</v>
-      </c>
-      <c r="F70" t="n">
-        <v>33566</v>
-      </c>
+        <v>1970</v>
+      </c>
+      <c r="E70" t="inlineStr"/>
+      <c r="F70" t="inlineStr"/>
       <c r="G70" t="n">
-        <v>109</v>
-      </c>
-      <c r="H70" t="n">
-        <v>13979</v>
-      </c>
+        <v>380</v>
+      </c>
+      <c r="H70" t="inlineStr"/>
       <c r="I70" t="n">
-        <v>22.88492472710245</v>
+        <v>17.0953</v>
       </c>
       <c r="J70" t="n">
-        <v>0.2472409829726473</v>
+        <v>0.3308090915150982</v>
       </c>
       <c r="K70" t="n">
-        <v>2.9899</v>
+        <v>1.665838405572881</v>
       </c>
       <c r="L70" t="n">
-        <v>204.5871559633028</v>
-      </c>
-      <c r="M70" t="inlineStr"/>
+        <v>286.6842105263158</v>
+      </c>
+      <c r="M70" t="n">
+        <v>14.2003</v>
+      </c>
       <c r="N70" t="inlineStr"/>
       <c r="O70" t="inlineStr"/>
-      <c r="P70" t="n">
-        <v>27.25</v>
-      </c>
+      <c r="P70" t="inlineStr"/>
       <c r="Q70" t="inlineStr"/>
       <c r="R70" t="inlineStr"/>
       <c r="S70" t="inlineStr"/>
       <c r="T70" t="inlineStr"/>
       <c r="U70" t="inlineStr"/>
       <c r="V70" t="inlineStr"/>
-      <c r="W70" t="inlineStr"/>
+      <c r="W70" t="n">
+        <v>284</v>
+      </c>
       <c r="X70" t="inlineStr"/>
-      <c r="Y70" t="n">
-        <v>8.4</v>
-      </c>
+      <c r="Y70" t="inlineStr"/>
       <c r="Z70" t="n">
-        <v>1.032222222222222</v>
-      </c>
-      <c r="AA70" t="inlineStr"/>
-      <c r="AB70" t="inlineStr"/>
+        <v>169567.8746222493</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -5979,121 +5677,177 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>MD-11</t>
+          <t>DC9-10</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>Wide</t>
+          <t>Narrow</t>
         </is>
       </c>
       <c r="D71" t="n">
-        <v>1990</v>
+        <v>1965</v>
       </c>
       <c r="E71" t="n">
-        <v>276691</v>
+        <v>41141</v>
       </c>
       <c r="F71" t="n">
-        <v>195045</v>
+        <v>33566</v>
       </c>
       <c r="G71" t="n">
-        <v>410</v>
+        <v>109</v>
       </c>
       <c r="H71" t="n">
-        <v>144782</v>
+        <v>13979</v>
       </c>
       <c r="I71" t="n">
-        <v>17.17456583460847</v>
+        <v>22.88492472710245</v>
       </c>
       <c r="J71" t="n">
-        <v>0.329294025279972</v>
+        <v>0.2472409829726473</v>
       </c>
       <c r="K71" t="n">
-        <v>1.744608638314735</v>
+        <v>2.9899</v>
       </c>
       <c r="L71" t="n">
-        <v>317.4756097560976</v>
-      </c>
-      <c r="M71" t="n">
-        <v>17.18295849059495</v>
-      </c>
+        <v>204.5871559633028</v>
+      </c>
+      <c r="M71" t="inlineStr"/>
       <c r="N71" t="inlineStr"/>
       <c r="O71" t="inlineStr"/>
-      <c r="P71" t="inlineStr"/>
-      <c r="Q71" t="n">
-        <v>0.7918255422774546</v>
-      </c>
-      <c r="R71" t="n">
-        <v>0.4158827258454688</v>
-      </c>
+      <c r="P71" t="n">
+        <v>27.25</v>
+      </c>
+      <c r="Q71" t="inlineStr"/>
+      <c r="R71" t="inlineStr"/>
       <c r="S71" t="inlineStr"/>
       <c r="T71" t="inlineStr"/>
       <c r="U71" t="inlineStr"/>
       <c r="V71" t="inlineStr"/>
-      <c r="W71" t="n">
-        <v>1.674345709353589</v>
-      </c>
+      <c r="W71" t="inlineStr"/>
       <c r="X71" t="n">
-        <v>254</v>
-      </c>
-      <c r="Y71" t="inlineStr"/>
-      <c r="Z71" t="n">
-        <v>4.8</v>
-      </c>
-      <c r="AA71" t="n">
-        <v>160911.0912490309</v>
-      </c>
-      <c r="AB71" t="n">
-        <v>1.037277585794662</v>
-      </c>
+        <v>8.4</v>
+      </c>
+      <c r="Y71" t="n">
+        <v>1.032222222222222</v>
+      </c>
+      <c r="Z71" t="inlineStr"/>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t xml:space="preserve">Saab-Fairchild </t>
+          <t xml:space="preserve">McDonnell Douglas </t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>340/B</t>
+          <t>MD-11</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>Regional</t>
+          <t>Wide</t>
         </is>
       </c>
       <c r="D72" t="n">
-        <v>1984</v>
-      </c>
-      <c r="E72" t="inlineStr"/>
-      <c r="F72" t="inlineStr"/>
+        <v>1990</v>
+      </c>
+      <c r="E72" t="n">
+        <v>276691</v>
+      </c>
+      <c r="F72" t="n">
+        <v>195045</v>
+      </c>
       <c r="G72" t="n">
-        <v>34</v>
-      </c>
-      <c r="H72" t="inlineStr"/>
-      <c r="I72" t="inlineStr"/>
-      <c r="J72" t="inlineStr"/>
-      <c r="K72" t="inlineStr"/>
+        <v>410</v>
+      </c>
+      <c r="H72" t="n">
+        <v>144782</v>
+      </c>
+      <c r="I72" t="n">
+        <v>17.17456583460847</v>
+      </c>
+      <c r="J72" t="n">
+        <v>0.329294025279972</v>
+      </c>
+      <c r="K72" t="n">
+        <v>1.744608638314735</v>
+      </c>
       <c r="L72" t="n">
-        <v>241.9117647058823</v>
-      </c>
-      <c r="M72" t="inlineStr"/>
+        <v>317.4756097560976</v>
+      </c>
+      <c r="M72" t="n">
+        <v>17.18295849059495</v>
+      </c>
       <c r="N72" t="inlineStr"/>
       <c r="O72" t="inlineStr"/>
       <c r="P72" t="inlineStr"/>
-      <c r="Q72" t="inlineStr"/>
-      <c r="R72" t="inlineStr"/>
+      <c r="Q72" t="n">
+        <v>0.7918255422774546</v>
+      </c>
+      <c r="R72" t="n">
+        <v>0.4158827258454688</v>
+      </c>
       <c r="S72" t="inlineStr"/>
       <c r="T72" t="inlineStr"/>
       <c r="U72" t="inlineStr"/>
       <c r="V72" t="inlineStr"/>
-      <c r="W72" t="inlineStr"/>
+      <c r="W72" t="n">
+        <v>254</v>
+      </c>
       <c r="X72" t="inlineStr"/>
-      <c r="Y72" t="inlineStr"/>
-      <c r="Z72" t="inlineStr"/>
-      <c r="AA72" t="inlineStr"/>
-      <c r="AB72" t="inlineStr"/>
+      <c r="Y72" t="n">
+        <v>4.8</v>
+      </c>
+      <c r="Z72" t="n">
+        <v>160911.0912490309</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Saab-Fairchild </t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>340/B</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>Regional</t>
+        </is>
+      </c>
+      <c r="D73" t="n">
+        <v>1984</v>
+      </c>
+      <c r="E73" t="inlineStr"/>
+      <c r="F73" t="inlineStr"/>
+      <c r="G73" t="n">
+        <v>34</v>
+      </c>
+      <c r="H73" t="inlineStr"/>
+      <c r="I73" t="inlineStr"/>
+      <c r="J73" t="inlineStr"/>
+      <c r="K73" t="inlineStr"/>
+      <c r="L73" t="n">
+        <v>241.9117647058823</v>
+      </c>
+      <c r="M73" t="inlineStr"/>
+      <c r="N73" t="inlineStr"/>
+      <c r="O73" t="inlineStr"/>
+      <c r="P73" t="inlineStr"/>
+      <c r="Q73" t="inlineStr"/>
+      <c r="R73" t="inlineStr"/>
+      <c r="S73" t="inlineStr"/>
+      <c r="T73" t="inlineStr"/>
+      <c r="U73" t="inlineStr"/>
+      <c r="V73" t="inlineStr"/>
+      <c r="W73" t="inlineStr"/>
+      <c r="X73" t="inlineStr"/>
+      <c r="Y73" t="inlineStr"/>
+      <c r="Z73" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>